<commit_message>
[IMP] procurement result template
</commit_message>
<xml_diff>
--- a/pabi_procurement_report/xlsx_template/xlsx_report_pabi_procurement_result.xlsx
+++ b/pabi_procurement_report/xlsx_template/xlsx_report_pabi_procurement_result.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3940" yWindow="7660" windowWidth="22480" windowHeight="10000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Budget Summary Report" sheetId="1" r:id="rId1"/>
@@ -75,13 +75,13 @@
     <t>เลขที่ PO</t>
   </si>
   <si>
-    <t>item</t>
-  </si>
-  <si>
-    <t>Asset Value</t>
-  </si>
-  <si>
-    <t>PO Total</t>
+    <t>ยอดรวมการจัดซื้อ</t>
+  </si>
+  <si>
+    <t>มูลค่าครุภัณฑ์</t>
+  </si>
+  <si>
+    <t>ครุภัณฑ์</t>
   </si>
 </sst>
 </file>
@@ -451,7 +451,7 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -509,13 +509,13 @@
         <v>13</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>10</v>

</xml_diff>